<commit_message>
finished graph for part 1
</commit_message>
<xml_diff>
--- a/olderbeef.xlsx
+++ b/olderbeef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbeausimon/Documents/RStudio_Files/eocps3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7DF57E5-53E6-1942-BF7A-C127FA3F14AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937B512C-28A1-464F-B9E2-23305100F60A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="1960" windowWidth="24240" windowHeight="13500" xr2:uid="{25FCE64A-C59E-E046-A737-82F6656546C2}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Per capita availability: Retail</t>
   </si>
   <si>
-    <t>Per capita availability: Boneless</t>
-  </si>
-  <si>
     <t>Total availability : Carcass</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Nonfood use: Ending stocks4</t>
+  </si>
+  <si>
+    <t>percapconsumption</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:R122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,34 +476,34 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -512,13 +512,13 @@
         <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
         <v>16</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
       </c>
       <c r="R1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
added more written questions and the model for the last question
</commit_message>
<xml_diff>
--- a/olderbeef.xlsx
+++ b/olderbeef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbeausimon/Documents/RStudio_Files/eocps3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937B512C-28A1-464F-B9E2-23305100F60A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9263AAB-8507-4547-A638-B7BA0DF4C13A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="1960" windowWidth="24240" windowHeight="13500" xr2:uid="{25FCE64A-C59E-E046-A737-82F6656546C2}"/>
   </bookViews>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA00687-2C76-164C-BF79-D3E4511426CC}">
   <dimension ref="A1:R122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added a total consumption column and model to q1
</commit_message>
<xml_diff>
--- a/olderbeef.xlsx
+++ b/olderbeef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbeausimon/Documents/RStudio_Files/eocps3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9263AAB-8507-4547-A638-B7BA0DF4C13A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28F2012-DF53-5948-8196-F5EAA77565CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="1960" windowWidth="24240" windowHeight="13500" xr2:uid="{25FCE64A-C59E-E046-A737-82F6656546C2}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>Total availability : Retail</t>
   </si>
   <si>
-    <t>Total availability : Boneless</t>
-  </si>
-  <si>
     <t>Factors for converting carcass weight to retail</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>percapconsumption</t>
+  </si>
+  <si>
+    <t>totalconsumption</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA00687-2C76-164C-BF79-D3E4511426CC}">
   <dimension ref="A1:R122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,25 +476,25 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>
@@ -503,7 +503,7 @@
         <v>13</v>
       </c>
       <c r="L1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -512,13 +512,13 @@
         <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>1</v>

</xml_diff>